<commit_message>
Backup folder - 2023-12-20 18:15:06
</commit_message>
<xml_diff>
--- a/АСД/РР1/Заміри часу виконання в залежності від числа елементів і початкового виду масиву.xlsx
+++ b/АСД/РР1/Заміри часу виконання в залежності від числа елементів і початкового виду масиву.xlsx
@@ -8,13 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yarik/Desktop/✈️ ХАІ 💻/АСД/РР1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE1D7C4-937A-3B47-A668-09E5B6AADE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F85C30-800A-1446-8452-E75359ED8BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12420" yWindow="4640" windowWidth="17820" windowHeight="13340" xr2:uid="{3EAAFC5D-F309-1E4B-8FCC-6D0771D8C019}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$B$2:$B$3</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$B$4:$B$9</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Лист1!$C$2:$C$3</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Лист1!$C$4:$C$9</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Лист1!$D$2:$D$3</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Лист1!$D$4:$D$9</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Лист1!$E$2:$E$3</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Лист1!$E$4:$E$9</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$C$2:$C$3</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$C$4:$C$9</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Лист1!$D$2:$D$3</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Лист1!$D$4:$D$9</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Лист1!$E$2:$E$3</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Лист1!$E$4:$E$9</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Лист1!$B$2:$B$3</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Лист1!$B$4:$B$9</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -231,6 +249,1048 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Заміри часу виконання в залежності від числа елементів і початкового виду масиву</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$2:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Затрачений час, од.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Випадковий порядок</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>301239</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>276334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1777222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1442161</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4183835</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3268229</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3E43-C743-92D0-2A6AEF517AD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$2:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Затрачений час, од.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Вже відсортовано</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>200161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>181592</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1243713</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1067728</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2822698</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2422996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3E43-C743-92D0-2A6AEF517AD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$2:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Затрачений час, од.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Зворотній порядок</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$E$4:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>191792</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170351</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1250146</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1109614</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2872916</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2431061</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3E43-C743-92D0-2A6AEF517AD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="300657520"/>
+        <c:axId val="334650864"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="300657520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334650864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="334650864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="300657520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-UA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8505EBD4-CCC7-8D33-4086-86B48511D542}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -530,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B503AAC0-66CE-5B41-826A-8F43AB413744}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,5 +1737,6 @@
     <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup folder - 2023-12-20 19:03:32
</commit_message>
<xml_diff>
--- a/АСД/РР1/Заміри часу виконання в залежності від числа елементів і початкового виду масиву.xlsx
+++ b/АСД/РР1/Заміри часу виконання в залежності від числа елементів і початкового виду масиву.xlsx
@@ -8,31 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yarik/Desktop/✈️ ХАІ 💻/АСД/РР1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F85C30-800A-1446-8452-E75359ED8BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118BAF55-16F3-264C-85BF-F03C019772F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="4640" windowWidth="17820" windowHeight="13340" xr2:uid="{3EAAFC5D-F309-1E4B-8FCC-6D0771D8C019}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="13400" windowHeight="11580" xr2:uid="{3EAAFC5D-F309-1E4B-8FCC-6D0771D8C019}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$B$2:$B$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$B$4:$B$9</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Лист1!$C$2:$C$3</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Лист1!$C$4:$C$9</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Лист1!$D$2:$D$3</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Лист1!$D$4:$D$9</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Лист1!$E$2:$E$3</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Лист1!$E$4:$E$9</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$C$2:$C$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$C$4:$C$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Лист1!$D$2:$D$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Лист1!$D$4:$D$9</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Лист1!$E$2:$E$3</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Лист1!$E$4:$E$9</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Лист1!$B$2:$B$3</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Лист1!$B$4:$B$9</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -80,7 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +77,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -196,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,12 +200,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -231,6 +215,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -352,6 +339,33 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Лист1!$C$4:$C$9</c:f>
@@ -412,6 +426,33 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Лист1!$D$4:$D$9</c:f>
@@ -472,6 +513,33 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Лист1!$E$4:$E$9</c:f>
@@ -525,6 +593,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1254,16 +1323,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1590,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B503AAC0-66CE-5B41-826A-8F43AB413744}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1612,22 +1681,22 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1635,16 +1704,16 @@
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="11">
         <v>10000</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>301239</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>200161</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>191792</v>
       </c>
     </row>
@@ -1652,14 +1721,16 @@
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="12">
+      <c r="B5" s="11">
+        <v>10000</v>
+      </c>
+      <c r="C5" s="10">
         <v>276334</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>181592</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>170351</v>
       </c>
     </row>
@@ -1667,16 +1738,16 @@
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="11">
         <v>50000</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>1777222</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>1243713</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>1250146</v>
       </c>
     </row>
@@ -1684,14 +1755,16 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="12">
+      <c r="B7" s="11">
+        <v>50000</v>
+      </c>
+      <c r="C7" s="10">
         <v>1442161</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>1067728</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>1109614</v>
       </c>
     </row>
@@ -1699,16 +1772,16 @@
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="11">
         <v>100000</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>4183835</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>2822698</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>2872916</v>
       </c>
     </row>
@@ -1716,25 +1789,24 @@
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="12">
+      <c r="B9" s="11">
+        <v>100000</v>
+      </c>
+      <c r="C9" s="10">
         <v>3268229</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <v>2422996</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>2431061</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B8:B9"/>
+  <mergeCells count="3">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>